<commit_message>
Sample image is added. \n Display the output in console
</commit_message>
<xml_diff>
--- a/src/main/resources/SampleData.xlsx
+++ b/src/main/resources/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
   <si>
     <t xml:space="preserve">sample1</t>
   </si>
@@ -41,9 +41,15 @@
     <t xml:space="preserve">sample121</t>
   </si>
   <si>
+    <t xml:space="preserve">Manish</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample122</t>
   </si>
   <si>
+    <t xml:space="preserve">Dua</t>
+  </si>
+  <si>
     <t xml:space="preserve">}</t>
   </si>
   <si>
@@ -53,12 +59,21 @@
     <t xml:space="preserve">sample2</t>
   </si>
   <si>
+    <t xml:space="preserve">[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dummy</t>
   </si>
   <si>
-    <t xml:space="preserve">[</t>
-  </si>
-  <si>
     <t xml:space="preserve">data1</t>
   </si>
   <si>
@@ -68,9 +83,6 @@
     <t xml:space="preserve">data3</t>
   </si>
   <si>
-    <t xml:space="preserve">]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[{</t>
   </si>
   <si>
@@ -81,9 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample3</t>
   </si>
   <si>
     <t xml:space="preserve">sample4</t>
@@ -250,11 +259,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -283,10 +292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -307,7 +316,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>6786868</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,40 +331,69 @@
       <c r="D5" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <v>12312</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1"/>
+      <c r="C12" s="2" t="n">
+        <v>123</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="2"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="3"/>
@@ -398,35 +436,35 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -461,15 +499,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,7 +527,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -510,7 +548,7 @@
   </sheetPr>
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -526,33 +564,33 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,53 +605,53 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="2" t="b">
+      <c r="C19" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>1</v>
@@ -621,15 +659,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>1</v>
@@ -637,12 +675,12 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>1</v>
@@ -650,40 +688,40 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -744,50 +782,50 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -795,7 +833,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -803,7 +841,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>3</v>
@@ -811,22 +849,22 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>1</v>
@@ -834,24 +872,24 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>10</v>
@@ -859,20 +897,20 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>1</v>
@@ -880,25 +918,25 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>1</v>
@@ -906,17 +944,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>1</v>
@@ -924,7 +962,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>2.3</v>
@@ -932,7 +970,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>3.4</v>
@@ -940,20 +978,20 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,12 +1006,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>